<commit_message>
Added event names and types in event table, some event notes
</commit_message>
<xml_diff>
--- a/Event Table/EventTable.xlsx
+++ b/Event Table/EventTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nagoya\Documents\Uni\Semester 2\SAM 2021\modellingAssignment1\Event Table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A541E51-2031-47D1-AF35-F10C33FC28D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE37970E-122A-4390-8FCC-37F6B142C35B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="15435" xr2:uid="{32C6574B-FC3F-4F92-B702-88451B0D3896}"/>
+    <workbookView xWindow="75" yWindow="390" windowWidth="31830" windowHeight="15435" xr2:uid="{32C6574B-FC3F-4F92-B702-88451B0D3896}"/>
   </bookViews>
   <sheets>
     <sheet name="eventTable" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="93">
   <si>
     <t>Event Name</t>
   </si>
@@ -227,13 +227,100 @@
   </si>
   <si>
     <t>Payslip email is sent to employees that opted in for notifications</t>
+  </si>
+  <si>
+    <t>Submit Customer Information</t>
+  </si>
+  <si>
+    <t>Submit Business Customer Information</t>
+  </si>
+  <si>
+    <t>ActiveGo System</t>
+  </si>
+  <si>
+    <t>ActiveGo System Developers</t>
+  </si>
+  <si>
+    <t>ActiveGo Management</t>
+  </si>
+  <si>
+    <t>ActiveGo Customer Interactions</t>
+  </si>
+  <si>
+    <t>ATO</t>
+  </si>
+  <si>
+    <t>Customers</t>
+  </si>
+  <si>
+    <t>Business Customers</t>
+  </si>
+  <si>
+    <t>Edit Customer Information</t>
+  </si>
+  <si>
+    <t>Edit Business Customer Information</t>
+  </si>
+  <si>
+    <t>Calculate Customer Hire Cost</t>
+  </si>
+  <si>
+    <t>Charge Customer for Hire and Deposit</t>
+  </si>
+  <si>
+    <t>Calculate Customer Deposit</t>
+  </si>
+  <si>
+    <t>Submit Customer Return</t>
+  </si>
+  <si>
+    <t>Submit Customer Hire</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Includes: First Name, Last Name, Postal Address, Email Address, Phone Number, Date of Birth</t>
+  </si>
+  <si>
+    <t>Includes: Company Name, Postal Address, Email Address, Phone Number</t>
+  </si>
+  <si>
+    <t>Includes: Actual Return Date, Pack Type, Pack Drop-Off Location, Pack Return Condition</t>
+  </si>
+  <si>
+    <t>Includes: Hire Date, Return Due Date, Pack Type, Pack Pickup Location, Pack Pickup Condition</t>
+  </si>
+  <si>
+    <t>Hold Customer Deposit</t>
+  </si>
+  <si>
+    <t>Release Customer Deposit</t>
+  </si>
+  <si>
+    <t>Charge Customer Late Fees</t>
+  </si>
+  <si>
+    <t>Calculate Customer Late Fees</t>
+  </si>
+  <si>
+    <t>Send Transaction Data to Bank</t>
+  </si>
+  <si>
+    <t>Customers via Customer Interactions</t>
+  </si>
+  <si>
+    <t>Business Customers via Customer Interactions</t>
+  </si>
+  <si>
+    <t>Customer Interactions</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -256,8 +343,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -312,6 +405,42 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF4F4F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE604BB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF18D6F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -353,7 +482,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -402,12 +531,85 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF18D6F0"/>
+      <color rgb="FFE604BB"/>
+      <color rgb="FFFF4F4F"/>
+      <color rgb="FFD0F7FC"/>
+      <color rgb="FFFBD1F3"/>
+      <color rgb="FFFCD4D0"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -716,25 +918,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{691D4392-63F1-4651-BDBD-40240F036054}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.140625" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" customWidth="1"/>
-    <col min="4" max="4" width="29.28515625" customWidth="1"/>
-    <col min="5" max="5" width="27.5703125" customWidth="1"/>
-    <col min="6" max="6" width="30.140625" customWidth="1"/>
-    <col min="7" max="7" width="28" customWidth="1"/>
-    <col min="8" max="8" width="30.28515625" customWidth="1"/>
+    <col min="1" max="1" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.5703125" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.28515625" style="38" customWidth="1"/>
+    <col min="5" max="5" width="27.5703125" style="38" customWidth="1"/>
+    <col min="6" max="6" width="30.140625" style="38" customWidth="1"/>
+    <col min="7" max="7" width="28" style="38" customWidth="1"/>
+    <col min="8" max="8" width="30.28515625" style="38" customWidth="1"/>
+    <col min="9" max="9" width="47.5703125" style="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -759,186 +962,438 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="17"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
+      <c r="I1" s="19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" s="35"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" s="35"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="D7" s="35"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" s="35"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="18"/>
+    </row>
+    <row r="9" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" s="35"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="18"/>
+    </row>
+    <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="18"/>
+    </row>
+    <row r="11" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="18"/>
+    </row>
+    <row r="12" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="18"/>
+    </row>
+    <row r="13" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="18"/>
+    </row>
+    <row r="14" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="18"/>
+    </row>
+    <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B15" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="18"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="23"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="26"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="23"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="26"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="23"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" s="37"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="26"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="23"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" s="37"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="36"/>
+      <c r="I19" s="26"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="23"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="36"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="36"/>
+      <c r="I20" s="26"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="23"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="36"/>
+      <c r="I21" s="26"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="23"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="36"/>
+      <c r="I22" s="26"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="23"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" s="37"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="36"/>
+      <c r="I23" s="26"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="23"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="36"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="36"/>
+      <c r="I24" s="26"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="23"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="36"/>
+      <c r="G25" s="36"/>
+      <c r="H25" s="36"/>
+      <c r="I25" s="26"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="23"/>
+      <c r="B26" s="24"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="36"/>
+      <c r="I26" s="26"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="23"/>
+      <c r="B27" s="24"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="26"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="23"/>
+      <c r="B28" s="24"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="36"/>
+      <c r="H28" s="36"/>
+      <c r="I28" s="26"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="23"/>
+      <c r="B29" s="24"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="36"/>
+      <c r="G29" s="36"/>
+      <c r="H29" s="36"/>
+      <c r="I29" s="26"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="23"/>
+      <c r="B30" s="24"/>
+      <c r="D30" s="37"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="36"/>
+      <c r="G30" s="36"/>
+      <c r="H30" s="36"/>
+      <c r="I30" s="26"/>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
More work on event table
</commit_message>
<xml_diff>
--- a/Event Table/EventTable.xlsx
+++ b/Event Table/EventTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nagoya\Documents\Uni\Semester 2\SAM 2021\modellingAssignment1\Event Table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE37970E-122A-4390-8FCC-37F6B142C35B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64D31E9C-A6FF-4535-95A2-57D120A7BCC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="75" yWindow="390" windowWidth="31830" windowHeight="15435" xr2:uid="{32C6574B-FC3F-4F92-B702-88451B0D3896}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{32C6574B-FC3F-4F92-B702-88451B0D3896}"/>
   </bookViews>
   <sheets>
     <sheet name="eventTable" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="136">
   <si>
     <t>Event Name</t>
   </si>
@@ -232,42 +232,12 @@
     <t>Submit Customer Information</t>
   </si>
   <si>
-    <t>Submit Business Customer Information</t>
-  </si>
-  <si>
-    <t>ActiveGo System</t>
-  </si>
-  <si>
-    <t>ActiveGo System Developers</t>
-  </si>
-  <si>
-    <t>ActiveGo Management</t>
-  </si>
-  <si>
-    <t>ActiveGo Customer Interactions</t>
-  </si>
-  <si>
-    <t>ATO</t>
-  </si>
-  <si>
-    <t>Customers</t>
-  </si>
-  <si>
-    <t>Business Customers</t>
-  </si>
-  <si>
     <t>Edit Customer Information</t>
   </si>
   <si>
-    <t>Edit Business Customer Information</t>
-  </si>
-  <si>
     <t>Calculate Customer Hire Cost</t>
   </si>
   <si>
-    <t>Charge Customer for Hire and Deposit</t>
-  </si>
-  <si>
     <t>Calculate Customer Deposit</t>
   </si>
   <si>
@@ -314,6 +284,165 @@
   </si>
   <si>
     <t>Customer Interactions</t>
+  </si>
+  <si>
+    <t>Customer Interactions enters customer's request for an equipment pack</t>
+  </si>
+  <si>
+    <t>Customer Interactions enters conformation of equipment pack return</t>
+  </si>
+  <si>
+    <t>Customer Interactions edits business customer information</t>
+  </si>
+  <si>
+    <t>Customer Interactions edits customer information</t>
+  </si>
+  <si>
+    <t>Customer Interactions inputs business customer information</t>
+  </si>
+  <si>
+    <t>Customer Interactions inputs customer information</t>
+  </si>
+  <si>
+    <t>Event output (Submit Customer Hire) is submitted to the ActiveGo system</t>
+  </si>
+  <si>
+    <t>Withhold Customer Deposit</t>
+  </si>
+  <si>
+    <t>Event (Submit Customer Return) "Pack Return Condition" parameter is (Incomplete/Damaged)</t>
+  </si>
+  <si>
+    <t>Event (Submit Customer Return) "Pack Return Condition" parameter is (Complete/Undamaged)</t>
+  </si>
+  <si>
+    <t>Event (Submit Customer Hire) "Return Due Date" parameter is equal to the value of the parameter +1 day</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>Trigger</t>
+  </si>
+  <si>
+    <t>Response</t>
+  </si>
+  <si>
+    <t>Destination</t>
+  </si>
+  <si>
+    <t>Event (Calculate Customer Late Fees) was triggered exactly 1 day prior</t>
+  </si>
+  <si>
+    <t>Event (Submit Customer Return) "Actual Return Date" is the current date</t>
+  </si>
+  <si>
+    <t>Charge Customer Hire and Deposit</t>
+  </si>
+  <si>
+    <t>Event(s) [Charge Customer Hire and Deposit | Charge Customer Late Fees] is/are triggered</t>
+  </si>
+  <si>
+    <t>Customer is not a business customer</t>
+  </si>
+  <si>
+    <t>Customer is a business customer</t>
+  </si>
+  <si>
+    <t>1. Store all input customer information on ActiveGo System</t>
+  </si>
+  <si>
+    <t>1. Store all input equipment hire information on the ActiveGo System</t>
+  </si>
+  <si>
+    <t>1. Store all new edited customer information on the ActiveGo System 2. Replace all previous customer information with current customer information</t>
+  </si>
+  <si>
+    <t>1. Store all input equipment return information on the ActiveGo System</t>
+  </si>
+  <si>
+    <t>1. Retrieve "Pack Type" parameter 2. Calculate daily fee in accordance with "Pack Type" parameter</t>
+  </si>
+  <si>
+    <t>1. Retrieve "Pack Type" parameter 2. Calculate deposit in accordance with "Pack Type" parameter</t>
+  </si>
+  <si>
+    <t>Event (Charge Customer Hire and Deposit) is completed</t>
+  </si>
+  <si>
+    <t>Event (Calculate Customer Deposit) is completed</t>
+  </si>
+  <si>
+    <t>Payment from Customer is received and transaction value is equivalent to calculated value of event (Charge Customer Hire and Deposit)</t>
+  </si>
+  <si>
+    <t>Customer Equipment Hire Collection</t>
+  </si>
+  <si>
+    <t>Customer Equipment Hire Return</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>Customer collects "Pack Type" from "Pack Pickup Location"</t>
+  </si>
+  <si>
+    <t>Customer returns "Pack Type" to "Pack Drop-Off Location"</t>
+  </si>
+  <si>
+    <t>Check Customer Payment Status</t>
+  </si>
+  <si>
+    <t>Payment from customer is approved by Bank</t>
+  </si>
+  <si>
+    <t>Payment from customer is declined by Bank</t>
+  </si>
+  <si>
+    <t>1. Retrieve value of events (Calculate Customer Hire Cost) and (Calculate Customer Deposit) 2. Send withdrawal request to Bank equal to total value of events</t>
+  </si>
+  <si>
+    <t>1. Send payment information to event (Hold Customer Deposit)</t>
+  </si>
+  <si>
+    <t>1. Store value of the event (Check Customer Payment Status)</t>
+  </si>
+  <si>
+    <t>1. Equipment Pack location is updated to the value of "Pack Drop-Off Location"</t>
+  </si>
+  <si>
+    <t>1. Equipment Pack location is updated to "Currently On Hire"</t>
+  </si>
+  <si>
+    <t>1. Display "Payment Declined" message 2. Prompt Customer Interactions to resolve payment issue with the Customer 3. Retry event or decline service</t>
+  </si>
+  <si>
+    <t>1. Do not initiate event (Release Customer Deposit) until Customer Interactions manually release the funds after the issue is resolved</t>
+  </si>
+  <si>
+    <t>1. Refund value of event (Calculate Customer Deposit) if event (Submit Customer Return) is complete and event (Withhold Customer Deposit) is not triggered</t>
+  </si>
+  <si>
+    <t>1. Store value of the event (Calculate Customer Hire Cost) 2. Multiply value by 1.5 3. Store multiplied value as "1 Day Late Fee"</t>
+  </si>
+  <si>
+    <t>1. Retrieve "1 Day Late Fee" 2. Add value of "1 Day Late Fee" to itself, and store that total as "2 Days Late Fee".</t>
+  </si>
+  <si>
+    <t>Event (Calculate Customer Late Fees) was triggered exactly 2 days prior</t>
+  </si>
+  <si>
+    <t>1. Retrieve "2 Days Late Fee". 2. Add value of "1 Day Late Fee" to "2 Days Late Fee". 3. Store new value as "3 Days Late Fee." 4. For all succeeding days, add the value calculated the previous day to the value of "1 Day Late Fee" and name the value "x Days Late Fee".</t>
+  </si>
+  <si>
+    <t>1. Retrieve most recently stored value of event (Calculate Customer Late Fees). 2. Charge customer the equivalent value.</t>
+  </si>
+  <si>
+    <t>1. Send transaction metadata to Bank</t>
   </si>
 </sst>
 </file>
@@ -350,7 +479,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -435,12 +564,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -482,7 +605,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -531,18 +654,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -576,15 +693,9 @@
     <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -593,6 +704,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -918,23 +1050,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{691D4392-63F1-4651-BDBD-40240F036054}">
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.5703125" style="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.28515625" style="38" customWidth="1"/>
-    <col min="5" max="5" width="27.5703125" style="38" customWidth="1"/>
-    <col min="6" max="6" width="30.140625" style="38" customWidth="1"/>
-    <col min="7" max="7" width="28" style="38" customWidth="1"/>
-    <col min="8" max="8" width="30.28515625" style="38" customWidth="1"/>
-    <col min="9" max="9" width="47.5703125" style="20" customWidth="1"/>
+    <col min="1" max="1" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34" style="34" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="124.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="120.140625" style="34" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" style="34" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="47.42578125" style="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -945,458 +1077,682 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>94</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="30" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="D2" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="E2" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="F2" s="36" t="s">
+        <v>105</v>
+      </c>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B3" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C3" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>104</v>
+      </c>
+      <c r="E3" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="F3" s="36" t="s">
+        <v>105</v>
+      </c>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A4" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="E4" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="F4" s="36" t="s">
+        <v>107</v>
+      </c>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A5" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" s="35" t="s">
+        <v>104</v>
+      </c>
+      <c r="E5" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="F5" s="36" t="s">
+        <v>107</v>
+      </c>
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="36" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="F6" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="F7" s="36" t="s">
+        <v>108</v>
+      </c>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="F8" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
+    </row>
+    <row r="9" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="F9" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="G9" s="36"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="36"/>
+    </row>
+    <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="37" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="F10" s="36" t="s">
+        <v>122</v>
+      </c>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="36"/>
+    </row>
+    <row r="11" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="37" t="s">
+        <v>119</v>
+      </c>
+      <c r="B11" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="E11" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="F11" s="36" t="s">
+        <v>123</v>
+      </c>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="36"/>
+    </row>
+    <row r="12" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="37" t="s">
+        <v>119</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="E12" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="F12" s="36" t="s">
+        <v>127</v>
+      </c>
+      <c r="G12" s="36"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="36"/>
+    </row>
+    <row r="13" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="31" t="s">
+        <v>113</v>
+      </c>
+      <c r="F13" s="36" t="s">
+        <v>124</v>
+      </c>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
+    </row>
+    <row r="14" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="18" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B3" s="29" t="s">
+      <c r="B14" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="F14" s="36" t="s">
+        <v>128</v>
+      </c>
+      <c r="G14" s="36"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="36"/>
+    </row>
+    <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="F15" s="36" t="s">
+        <v>129</v>
+      </c>
+      <c r="G15" s="36"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="36"/>
+    </row>
+    <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="37" t="s">
+        <v>114</v>
+      </c>
+      <c r="B16" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="32" t="s">
-        <v>91</v>
-      </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="18" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B4" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="31" t="s">
-        <v>92</v>
-      </c>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="18" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B5" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="31" t="s">
-        <v>92</v>
-      </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
-      <c r="I5" s="18" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B6" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="31" t="s">
-        <v>92</v>
-      </c>
-      <c r="D6" s="35"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="18" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B7" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="31" t="s">
-        <v>92</v>
-      </c>
-      <c r="D7" s="35"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="18" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B8" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="D8" s="35"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="18"/>
-    </row>
-    <row r="9" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B9" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="D9" s="35"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="18"/>
-    </row>
-    <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B10" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="31" t="s">
-        <v>92</v>
-      </c>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="18"/>
-    </row>
-    <row r="11" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B11" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="18"/>
-    </row>
-    <row r="12" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B12" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="18"/>
-    </row>
-    <row r="13" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B13" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="34"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="18"/>
-    </row>
-    <row r="14" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B14" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="31" t="s">
-        <v>92</v>
-      </c>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="18"/>
-    </row>
-    <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B15" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="18"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="23"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="36"/>
+      <c r="C16" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="D16" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="F16" s="36" t="s">
+        <v>126</v>
+      </c>
       <c r="G16" s="36"/>
       <c r="H16" s="36"/>
-      <c r="I16" s="26"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="23"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="36"/>
+      <c r="I16" s="36"/>
+    </row>
+    <row r="17" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="37" t="s">
+        <v>115</v>
+      </c>
+      <c r="B17" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="F17" s="36" t="s">
+        <v>125</v>
+      </c>
       <c r="G17" s="36"/>
       <c r="H17" s="36"/>
-      <c r="I17" s="26"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="23"/>
-      <c r="B18" s="24"/>
-      <c r="C18" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="D18" s="37"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="36"/>
+      <c r="I17" s="36"/>
+    </row>
+    <row r="18" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="F18" s="36" t="s">
+        <v>130</v>
+      </c>
       <c r="G18" s="36"/>
       <c r="H18" s="36"/>
-      <c r="I18" s="26"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="23"/>
-      <c r="B19" s="24"/>
-      <c r="C19" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="D19" s="37"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="36"/>
+      <c r="I18" s="36"/>
+    </row>
+    <row r="19" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="38" t="s">
+        <v>99</v>
+      </c>
+      <c r="F19" s="36" t="s">
+        <v>131</v>
+      </c>
       <c r="G19" s="36"/>
       <c r="H19" s="36"/>
-      <c r="I19" s="26"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="23"/>
-      <c r="B20" s="24"/>
-      <c r="C20" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="36"/>
+      <c r="I19" s="36"/>
+    </row>
+    <row r="20" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="38" t="s">
+        <v>132</v>
+      </c>
+      <c r="F20" s="36" t="s">
+        <v>133</v>
+      </c>
       <c r="G20" s="36"/>
       <c r="H20" s="36"/>
-      <c r="I20" s="26"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="23"/>
-      <c r="B21" s="24"/>
-      <c r="C21" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="36"/>
+      <c r="I20" s="36"/>
+    </row>
+    <row r="21" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="37" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="38" t="s">
+        <v>100</v>
+      </c>
+      <c r="F21" s="36" t="s">
+        <v>134</v>
+      </c>
       <c r="G21" s="36"/>
       <c r="H21" s="36"/>
-      <c r="I21" s="26"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="23"/>
-      <c r="B22" s="24"/>
-      <c r="C22" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="36"/>
+      <c r="I21" s="36"/>
+    </row>
+    <row r="22" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="B22" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="F22" s="36" t="s">
+        <v>135</v>
+      </c>
       <c r="G22" s="36"/>
       <c r="H22" s="36"/>
-      <c r="I22" s="26"/>
+      <c r="I22" s="36"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="23"/>
-      <c r="B23" s="24"/>
-      <c r="C23" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="D23" s="37"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="36"/>
-      <c r="I23" s="26"/>
+      <c r="A23" s="21"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="32"/>
+      <c r="I23" s="24"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="23"/>
-      <c r="B24" s="24"/>
-      <c r="C24" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="36"/>
-      <c r="I24" s="26"/>
+      <c r="A24" s="21"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="24"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="23"/>
-      <c r="B25" s="24"/>
-      <c r="C25" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="36"/>
-      <c r="H25" s="36"/>
-      <c r="I25" s="26"/>
+      <c r="A25" s="21"/>
+      <c r="B25" s="22"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="32"/>
+      <c r="I25" s="24"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="23"/>
-      <c r="B26" s="24"/>
-      <c r="D26" s="37"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="36"/>
-      <c r="I26" s="26"/>
+      <c r="A26" s="39"/>
+      <c r="B26" s="33"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="41"/>
+      <c r="G26" s="41"/>
+      <c r="H26" s="41"/>
+      <c r="I26" s="41"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="23"/>
-      <c r="B27" s="24"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="26"/>
+      <c r="A27" s="39"/>
+      <c r="B27" s="33"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="40"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="41"/>
+      <c r="G27" s="41"/>
+      <c r="H27" s="41"/>
+      <c r="I27" s="41"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="23"/>
-      <c r="B28" s="24"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="26"/>
+      <c r="A28" s="21"/>
+      <c r="B28" s="22"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="24"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="23"/>
-      <c r="B29" s="24"/>
-      <c r="D29" s="37"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="36"/>
-      <c r="I29" s="26"/>
+      <c r="A29" s="21"/>
+      <c r="B29" s="22"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="24"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="23"/>
-      <c r="B30" s="24"/>
-      <c r="D30" s="37"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="36"/>
-      <c r="G30" s="36"/>
-      <c r="H30" s="36"/>
-      <c r="I30" s="26"/>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="23"/>
+      <c r="A30" s="21"/>
+      <c r="B30" s="22"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="32"/>
+      <c r="H30" s="32"/>
+      <c r="I30" s="24"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="21"/>
+      <c r="B31" s="22"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="32"/>
+      <c r="G31" s="32"/>
+      <c r="H31" s="32"/>
+      <c r="I31" s="24"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="21"/>
+      <c r="B32" s="22"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="32"/>
+      <c r="G32" s="32"/>
+      <c r="H32" s="32"/>
+      <c r="I32" s="24"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="21"/>
+      <c r="B33" s="22"/>
+      <c r="D33" s="33"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="32"/>
+      <c r="I33" s="24"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="21"/>
+      <c r="B34" s="22"/>
+      <c r="D34" s="33"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="32"/>
+      <c r="G34" s="32"/>
+      <c r="H34" s="32"/>
+      <c r="I34" s="24"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="21"/>
+      <c r="B35" s="22"/>
+      <c r="D35" s="33"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="32"/>
+      <c r="G35" s="32"/>
+      <c r="H35" s="32"/>
+      <c r="I35" s="24"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="21"/>
+      <c r="B36" s="22"/>
+      <c r="D36" s="33"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="32"/>
+      <c r="G36" s="32"/>
+      <c r="H36" s="32"/>
+      <c r="I36" s="24"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="21"/>
+      <c r="B37" s="22"/>
+      <c r="D37" s="33"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="32"/>
+      <c r="G37" s="32"/>
+      <c r="H37" s="32"/>
+      <c r="I37" s="24"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Finished all columns in event table except for notes
</commit_message>
<xml_diff>
--- a/Event Table/EventTable.xlsx
+++ b/Event Table/EventTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nagoya\Documents\Uni\Semester 2\SAM 2021\modellingAssignment1\Event Table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64D31E9C-A6FF-4535-95A2-57D120A7BCC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9F45F7B-1818-43D6-8AF1-F7F56D6ADF1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{32C6574B-FC3F-4F92-B702-88451B0D3896}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="144">
   <si>
     <t>Event Name</t>
   </si>
@@ -358,18 +358,9 @@
     <t>1. Store all input equipment hire information on the ActiveGo System</t>
   </si>
   <si>
-    <t>1. Store all new edited customer information on the ActiveGo System 2. Replace all previous customer information with current customer information</t>
-  </si>
-  <si>
     <t>1. Store all input equipment return information on the ActiveGo System</t>
   </si>
   <si>
-    <t>1. Retrieve "Pack Type" parameter 2. Calculate daily fee in accordance with "Pack Type" parameter</t>
-  </si>
-  <si>
-    <t>1. Retrieve "Pack Type" parameter 2. Calculate deposit in accordance with "Pack Type" parameter</t>
-  </si>
-  <si>
     <t>Event (Charge Customer Hire and Deposit) is completed</t>
   </si>
   <si>
@@ -403,9 +394,6 @@
     <t>Payment from customer is declined by Bank</t>
   </si>
   <si>
-    <t>1. Retrieve value of events (Calculate Customer Hire Cost) and (Calculate Customer Deposit) 2. Send withdrawal request to Bank equal to total value of events</t>
-  </si>
-  <si>
     <t>1. Send payment information to event (Hold Customer Deposit)</t>
   </si>
   <si>
@@ -418,31 +406,80 @@
     <t>1. Equipment Pack location is updated to "Currently On Hire"</t>
   </si>
   <si>
-    <t>1. Display "Payment Declined" message 2. Prompt Customer Interactions to resolve payment issue with the Customer 3. Retry event or decline service</t>
-  </si>
-  <si>
     <t>1. Do not initiate event (Release Customer Deposit) until Customer Interactions manually release the funds after the issue is resolved</t>
   </si>
   <si>
     <t>1. Refund value of event (Calculate Customer Deposit) if event (Submit Customer Return) is complete and event (Withhold Customer Deposit) is not triggered</t>
   </si>
   <si>
-    <t>1. Store value of the event (Calculate Customer Hire Cost) 2. Multiply value by 1.5 3. Store multiplied value as "1 Day Late Fee"</t>
-  </si>
-  <si>
-    <t>1. Retrieve "1 Day Late Fee" 2. Add value of "1 Day Late Fee" to itself, and store that total as "2 Days Late Fee".</t>
-  </si>
-  <si>
     <t>Event (Calculate Customer Late Fees) was triggered exactly 2 days prior</t>
   </si>
   <si>
-    <t>1. Retrieve "2 Days Late Fee". 2. Add value of "1 Day Late Fee" to "2 Days Late Fee". 3. Store new value as "3 Days Late Fee." 4. For all succeeding days, add the value calculated the previous day to the value of "1 Day Late Fee" and name the value "x Days Late Fee".</t>
-  </si>
-  <si>
-    <t>1. Retrieve most recently stored value of event (Calculate Customer Late Fees). 2. Charge customer the equivalent value.</t>
-  </si>
-  <si>
     <t>1. Send transaction metadata to Bank</t>
+  </si>
+  <si>
+    <t>1. Store all new edited customer information on the ActiveGo System 
+2. Replace all previous customer information with current customer information</t>
+  </si>
+  <si>
+    <t>1. Retrieve "Pack Type" parameter 
+2. Calculate daily fee in accordance with "Pack Type" parameter</t>
+  </si>
+  <si>
+    <t>1. Retrieve "Pack Type" parameter 
+2. Calculate deposit in accordance with "Pack Type" parameter</t>
+  </si>
+  <si>
+    <t>1. Retrieve value of events (Calculate Customer Hire Cost) and (Calculate Customer Deposit) 
+2. Send withdrawal request to Bank equal to total value of events</t>
+  </si>
+  <si>
+    <t>1. Display "Payment Declined" message 
+2. Prompt Customer Interactions to resolve payment issue with the Customer 
+3. Retry event or decline service</t>
+  </si>
+  <si>
+    <t>1. Store value of the event (Calculate Customer Hire Cost) 
+2. Multiply value by 1.5 
+3. Store multiplied value as "1 Day Late Fee"</t>
+  </si>
+  <si>
+    <t>1. Retrieve "1 Day Late Fee" 
+2. Add value of "1 Day Late Fee" to itself, and store that total as "2 Days Late Fee"</t>
+  </si>
+  <si>
+    <t>1. Retrieve "2 Days Late Fee"
+2. Add value of "1 Day Late Fee" to "2 Days Late Fee"
+3. Store new value as "3 Days Late Fee" 
+4. For all succeeding days, add the value calculated the previous day to the value of "1 Day Late Fee" and name the value "x Days Late Fee"</t>
+  </si>
+  <si>
+    <t>1. Retrieve most recently stored value of event (Calculate Customer Late Fees)
+2. Charge customer the equivalent value</t>
+  </si>
+  <si>
+    <t>Display deposit status to Customer Interactions</t>
+  </si>
+  <si>
+    <t>Send fund transfer request to bank</t>
+  </si>
+  <si>
+    <t>Data stored in system</t>
+  </si>
+  <si>
+    <t>Display edit confirmation to Customer Interactions</t>
+  </si>
+  <si>
+    <t>Withdrawal request sent to bank</t>
+  </si>
+  <si>
+    <t>Send relevant transaction data to bank</t>
+  </si>
+  <si>
+    <t>ActiveGo System</t>
+  </si>
+  <si>
+    <t>Confirm bank has received funds, store value in the system</t>
   </si>
 </sst>
 </file>
@@ -693,9 +730,6 @@
     <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -714,9 +748,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
@@ -725,6 +756,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1052,8 +1089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{691D4392-63F1-4651-BDBD-40240F036054}">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1061,11 +1098,11 @@
     <col min="1" max="1" width="35.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34" style="34" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="124.5703125" style="34" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="120.140625" style="34" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" style="34" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" style="34" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34" style="33" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="69.5703125" style="33" customWidth="1"/>
+    <col min="6" max="6" width="135.85546875" style="33" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" style="33" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" style="33" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="47.42578125" style="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1098,8 +1135,8 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
+    <row r="2" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="36" t="s">
         <v>64</v>
       </c>
       <c r="B2" s="27" t="s">
@@ -1108,23 +1145,27 @@
       <c r="C2" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="E2" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="F2" s="36" t="s">
+      <c r="F2" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36" t="s">
+      <c r="G2" s="40" t="s">
+        <v>138</v>
+      </c>
+      <c r="H2" s="34" t="s">
+        <v>142</v>
+      </c>
+      <c r="I2" s="35" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
+    <row r="3" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="36" t="s">
         <v>64</v>
       </c>
       <c r="B3" s="27" t="s">
@@ -1133,23 +1174,27 @@
       <c r="C3" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="E3" s="31" t="s">
+      <c r="E3" s="35" t="s">
         <v>87</v>
       </c>
-      <c r="F3" s="36" t="s">
+      <c r="F3" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36" t="s">
+      <c r="G3" s="40" t="s">
+        <v>138</v>
+      </c>
+      <c r="H3" s="34" t="s">
+        <v>142</v>
+      </c>
+      <c r="I3" s="35" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A4" s="37" t="s">
+    <row r="4" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="36" t="s">
         <v>65</v>
       </c>
       <c r="B4" s="27" t="s">
@@ -1158,23 +1203,27 @@
       <c r="C4" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="D4" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="E4" s="31" t="s">
+      <c r="E4" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="F4" s="36" t="s">
-        <v>107</v>
-      </c>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36" t="s">
+      <c r="F4" s="35" t="s">
+        <v>127</v>
+      </c>
+      <c r="G4" s="40" t="s">
+        <v>139</v>
+      </c>
+      <c r="H4" s="34" t="s">
+        <v>142</v>
+      </c>
+      <c r="I4" s="35" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A5" s="37" t="s">
+    <row r="5" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="36" t="s">
         <v>65</v>
       </c>
       <c r="B5" s="27" t="s">
@@ -1183,23 +1232,27 @@
       <c r="C5" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="E5" s="31" t="s">
+      <c r="E5" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="F5" s="36" t="s">
-        <v>107</v>
-      </c>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="36" t="s">
+      <c r="F5" s="35" t="s">
+        <v>127</v>
+      </c>
+      <c r="G5" s="40" t="s">
+        <v>139</v>
+      </c>
+      <c r="H5" s="34" t="s">
+        <v>142</v>
+      </c>
+      <c r="I5" s="35" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="37" t="s">
+    <row r="6" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="36" t="s">
         <v>69</v>
       </c>
       <c r="B6" s="27" t="s">
@@ -1211,20 +1264,24 @@
       <c r="D6" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="31" t="s">
+      <c r="E6" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="F6" s="36" t="s">
+      <c r="F6" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="36" t="s">
+      <c r="G6" s="40" t="s">
+        <v>138</v>
+      </c>
+      <c r="H6" s="34" t="s">
+        <v>142</v>
+      </c>
+      <c r="I6" s="35" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="37" t="s">
+    <row r="7" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="36" t="s">
         <v>68</v>
       </c>
       <c r="B7" s="27" t="s">
@@ -1236,20 +1293,24 @@
       <c r="D7" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="31" t="s">
+      <c r="E7" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="F7" s="36" t="s">
-        <v>108</v>
-      </c>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="36" t="s">
+      <c r="F7" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="G7" s="40" t="s">
+        <v>138</v>
+      </c>
+      <c r="H7" s="34" t="s">
+        <v>142</v>
+      </c>
+      <c r="I7" s="35" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="37" t="s">
+    <row r="8" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="36" t="s">
         <v>66</v>
       </c>
       <c r="B8" s="26" t="s">
@@ -1261,18 +1322,22 @@
       <c r="D8" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="31" t="s">
+      <c r="E8" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="F8" s="36" t="s">
-        <v>109</v>
-      </c>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="36"/>
-    </row>
-    <row r="9" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="37" t="s">
+      <c r="F8" s="35" t="s">
+        <v>128</v>
+      </c>
+      <c r="G8" s="40" t="s">
+        <v>138</v>
+      </c>
+      <c r="H8" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="35"/>
+    </row>
+    <row r="9" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="36" t="s">
         <v>67</v>
       </c>
       <c r="B9" s="26" t="s">
@@ -1284,18 +1349,22 @@
       <c r="D9" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="31" t="s">
+      <c r="E9" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="F9" s="36" t="s">
-        <v>110</v>
-      </c>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="36"/>
-    </row>
-    <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="37" t="s">
+      <c r="F9" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="G9" s="40" t="s">
+        <v>138</v>
+      </c>
+      <c r="H9" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="35"/>
+    </row>
+    <row r="10" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="36" t="s">
         <v>101</v>
       </c>
       <c r="B10" s="26" t="s">
@@ -1307,19 +1376,23 @@
       <c r="D10" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="31" t="s">
-        <v>112</v>
-      </c>
-      <c r="F10" s="36" t="s">
-        <v>122</v>
-      </c>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="36"/>
-    </row>
-    <row r="11" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="37" t="s">
-        <v>119</v>
+      <c r="E10" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="F10" s="35" t="s">
+        <v>130</v>
+      </c>
+      <c r="G10" s="40" t="s">
+        <v>140</v>
+      </c>
+      <c r="H10" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="35"/>
+    </row>
+    <row r="11" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="36" t="s">
+        <v>116</v>
       </c>
       <c r="B11" s="26" t="s">
         <v>15</v>
@@ -1328,21 +1401,25 @@
         <v>10</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>120</v>
-      </c>
-      <c r="E11" s="31" t="s">
-        <v>111</v>
-      </c>
-      <c r="F11" s="36" t="s">
-        <v>123</v>
-      </c>
-      <c r="G11" s="36"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="36"/>
-    </row>
-    <row r="12" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="E11" s="35" t="s">
+        <v>108</v>
+      </c>
+      <c r="F11" s="35" t="s">
         <v>119</v>
+      </c>
+      <c r="G11" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="35"/>
+    </row>
+    <row r="12" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="36" t="s">
+        <v>116</v>
       </c>
       <c r="B12" s="26" t="s">
         <v>15</v>
@@ -1351,20 +1428,24 @@
         <v>10</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>121</v>
-      </c>
-      <c r="E12" s="31" t="s">
-        <v>111</v>
-      </c>
-      <c r="F12" s="36" t="s">
-        <v>127</v>
-      </c>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="36"/>
-    </row>
-    <row r="13" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="37" t="s">
+        <v>118</v>
+      </c>
+      <c r="E12" s="35" t="s">
+        <v>108</v>
+      </c>
+      <c r="F12" s="35" t="s">
+        <v>131</v>
+      </c>
+      <c r="G12" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" s="35"/>
+    </row>
+    <row r="13" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="36" t="s">
         <v>75</v>
       </c>
       <c r="B13" s="26" t="s">
@@ -1376,18 +1457,22 @@
       <c r="D13" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="31" t="s">
-        <v>113</v>
-      </c>
-      <c r="F13" s="36" t="s">
-        <v>124</v>
-      </c>
-      <c r="G13" s="36"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="36"/>
-    </row>
-    <row r="14" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="37" t="s">
+      <c r="E13" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="F13" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="G13" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="H13" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13" s="35"/>
+    </row>
+    <row r="14" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="36" t="s">
         <v>90</v>
       </c>
       <c r="B14" s="26" t="s">
@@ -1399,18 +1484,22 @@
       <c r="D14" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="31" t="s">
+      <c r="E14" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="F14" s="36" t="s">
-        <v>128</v>
-      </c>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="36"/>
-    </row>
-    <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="37" t="s">
+      <c r="F14" s="35" t="s">
+        <v>123</v>
+      </c>
+      <c r="G14" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="H14" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" s="35"/>
+    </row>
+    <row r="15" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="36" t="s">
         <v>76</v>
       </c>
       <c r="B15" s="26" t="s">
@@ -1422,64 +1511,76 @@
       <c r="D15" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="31" t="s">
+      <c r="E15" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="F15" s="36" t="s">
-        <v>129</v>
-      </c>
-      <c r="G15" s="36"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="36"/>
-    </row>
-    <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="37" t="s">
-        <v>114</v>
+      <c r="F15" s="35" t="s">
+        <v>124</v>
+      </c>
+      <c r="G15" s="40" t="s">
+        <v>137</v>
+      </c>
+      <c r="H15" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="I15" s="35"/>
+    </row>
+    <row r="16" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="36" t="s">
+        <v>111</v>
       </c>
       <c r="B16" s="27" t="s">
         <v>32</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D16" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="31" t="s">
-        <v>117</v>
-      </c>
-      <c r="F16" s="36" t="s">
-        <v>126</v>
-      </c>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="36"/>
-    </row>
-    <row r="17" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="37" t="s">
-        <v>115</v>
+      <c r="E16" s="35" t="s">
+        <v>114</v>
+      </c>
+      <c r="F16" s="35" t="s">
+        <v>122</v>
+      </c>
+      <c r="G16" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" s="34" t="s">
+        <v>142</v>
+      </c>
+      <c r="I16" s="35"/>
+    </row>
+    <row r="17" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="36" t="s">
+        <v>112</v>
       </c>
       <c r="B17" s="27" t="s">
         <v>32</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D17" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="E17" s="31" t="s">
-        <v>118</v>
-      </c>
-      <c r="F17" s="36" t="s">
-        <v>125</v>
-      </c>
-      <c r="G17" s="36"/>
-      <c r="H17" s="36"/>
-      <c r="I17" s="36"/>
-    </row>
-    <row r="18" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="37" t="s">
+      <c r="E17" s="35" t="s">
+        <v>115</v>
+      </c>
+      <c r="F17" s="35" t="s">
+        <v>121</v>
+      </c>
+      <c r="G17" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" s="34" t="s">
+        <v>142</v>
+      </c>
+      <c r="I17" s="35"/>
+    </row>
+    <row r="18" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="36" t="s">
         <v>78</v>
       </c>
       <c r="B18" s="25" t="s">
@@ -1491,18 +1592,22 @@
       <c r="D18" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="E18" s="38" t="s">
+      <c r="E18" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="F18" s="36" t="s">
-        <v>130</v>
-      </c>
-      <c r="G18" s="36"/>
-      <c r="H18" s="36"/>
-      <c r="I18" s="36"/>
-    </row>
-    <row r="19" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="37" t="s">
+      <c r="F18" s="35" t="s">
+        <v>132</v>
+      </c>
+      <c r="G18" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="I18" s="35"/>
+    </row>
+    <row r="19" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="36" t="s">
         <v>78</v>
       </c>
       <c r="B19" s="25" t="s">
@@ -1514,18 +1619,22 @@
       <c r="D19" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="38" t="s">
+      <c r="E19" s="40" t="s">
         <v>99</v>
       </c>
-      <c r="F19" s="36" t="s">
-        <v>131</v>
-      </c>
-      <c r="G19" s="36"/>
-      <c r="H19" s="36"/>
-      <c r="I19" s="36"/>
-    </row>
-    <row r="20" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="37" t="s">
+      <c r="F19" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="G19" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="I19" s="35"/>
+    </row>
+    <row r="20" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="36" t="s">
         <v>78</v>
       </c>
       <c r="B20" s="25" t="s">
@@ -1537,18 +1646,22 @@
       <c r="D20" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="E20" s="38" t="s">
-        <v>132</v>
-      </c>
-      <c r="F20" s="36" t="s">
-        <v>133</v>
-      </c>
-      <c r="G20" s="36"/>
-      <c r="H20" s="36"/>
-      <c r="I20" s="36"/>
-    </row>
-    <row r="21" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="37" t="s">
+      <c r="E20" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="F20" s="35" t="s">
+        <v>134</v>
+      </c>
+      <c r="G20" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="H20" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20" s="35"/>
+    </row>
+    <row r="21" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="36" t="s">
         <v>77</v>
       </c>
       <c r="B21" s="25" t="s">
@@ -1560,18 +1673,22 @@
       <c r="D21" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="E21" s="38" t="s">
+      <c r="E21" s="40" t="s">
         <v>100</v>
       </c>
-      <c r="F21" s="36" t="s">
-        <v>134</v>
-      </c>
-      <c r="G21" s="36"/>
-      <c r="H21" s="36"/>
-      <c r="I21" s="36"/>
-    </row>
-    <row r="22" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="37" t="s">
+      <c r="F21" s="35" t="s">
+        <v>135</v>
+      </c>
+      <c r="G21" s="40" t="s">
+        <v>140</v>
+      </c>
+      <c r="H21" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="I21" s="35"/>
+    </row>
+    <row r="22" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="36" t="s">
         <v>79</v>
       </c>
       <c r="B22" s="26" t="s">
@@ -1583,15 +1700,19 @@
       <c r="D22" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="E22" s="31" t="s">
+      <c r="E22" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="F22" s="36" t="s">
-        <v>135</v>
-      </c>
-      <c r="G22" s="36"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="36"/>
+      <c r="F22" s="35" t="s">
+        <v>126</v>
+      </c>
+      <c r="G22" s="40" t="s">
+        <v>141</v>
+      </c>
+      <c r="H22" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="I22" s="35"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="21"/>
@@ -1599,62 +1720,62 @@
       <c r="C23" s="23"/>
       <c r="D23" s="23"/>
       <c r="E23" s="23"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="32"/>
-      <c r="H23" s="32"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="31"/>
       <c r="I23" s="24"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="21"/>
       <c r="B24" s="22"/>
       <c r="C24" s="23"/>
-      <c r="D24" s="33"/>
+      <c r="D24" s="32"/>
       <c r="E24" s="23"/>
-      <c r="F24" s="32"/>
-      <c r="G24" s="32"/>
-      <c r="H24" s="32"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="31"/>
       <c r="I24" s="24"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="21"/>
       <c r="B25" s="22"/>
-      <c r="D25" s="33"/>
+      <c r="D25" s="32"/>
       <c r="E25" s="23"/>
-      <c r="F25" s="32"/>
-      <c r="G25" s="32"/>
-      <c r="H25" s="32"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="31"/>
       <c r="I25" s="24"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="39"/>
-      <c r="B26" s="33"/>
-      <c r="C26" s="40"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="41"/>
-      <c r="G26" s="41"/>
-      <c r="H26" s="41"/>
-      <c r="I26" s="41"/>
+      <c r="A26" s="37"/>
+      <c r="B26" s="32"/>
+      <c r="C26" s="38"/>
+      <c r="D26" s="38"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="39"/>
+      <c r="G26" s="39"/>
+      <c r="H26" s="39"/>
+      <c r="I26" s="39"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="39"/>
-      <c r="B27" s="33"/>
-      <c r="C27" s="40"/>
-      <c r="D27" s="40"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="41"/>
-      <c r="G27" s="41"/>
-      <c r="H27" s="41"/>
-      <c r="I27" s="41"/>
+      <c r="A27" s="37"/>
+      <c r="B27" s="32"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="39"/>
+      <c r="G27" s="39"/>
+      <c r="H27" s="39"/>
+      <c r="I27" s="39"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="21"/>
       <c r="B28" s="22"/>
       <c r="D28" s="23"/>
       <c r="E28" s="23"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="31"/>
+      <c r="H28" s="31"/>
       <c r="I28" s="24"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -1662,19 +1783,19 @@
       <c r="B29" s="22"/>
       <c r="D29" s="23"/>
       <c r="E29" s="23"/>
-      <c r="F29" s="32"/>
-      <c r="G29" s="32"/>
-      <c r="H29" s="32"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="31"/>
       <c r="I29" s="24"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="21"/>
       <c r="B30" s="22"/>
-      <c r="D30" s="33"/>
+      <c r="D30" s="32"/>
       <c r="E30" s="23"/>
-      <c r="F30" s="32"/>
-      <c r="G30" s="32"/>
-      <c r="H30" s="32"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="31"/>
       <c r="I30" s="24"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -1682,9 +1803,9 @@
       <c r="B31" s="22"/>
       <c r="D31" s="23"/>
       <c r="E31" s="23"/>
-      <c r="F31" s="32"/>
-      <c r="G31" s="32"/>
-      <c r="H31" s="32"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="31"/>
+      <c r="H31" s="31"/>
       <c r="I31" s="24"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -1692,59 +1813,59 @@
       <c r="B32" s="22"/>
       <c r="D32" s="23"/>
       <c r="E32" s="23"/>
-      <c r="F32" s="32"/>
-      <c r="G32" s="32"/>
-      <c r="H32" s="32"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="31"/>
+      <c r="H32" s="31"/>
       <c r="I32" s="24"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="21"/>
       <c r="B33" s="22"/>
-      <c r="D33" s="33"/>
+      <c r="D33" s="32"/>
       <c r="E33" s="23"/>
-      <c r="F33" s="32"/>
-      <c r="G33" s="32"/>
-      <c r="H33" s="32"/>
+      <c r="F33" s="31"/>
+      <c r="G33" s="31"/>
+      <c r="H33" s="31"/>
       <c r="I33" s="24"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="21"/>
       <c r="B34" s="22"/>
-      <c r="D34" s="33"/>
+      <c r="D34" s="32"/>
       <c r="E34" s="23"/>
-      <c r="F34" s="32"/>
-      <c r="G34" s="32"/>
-      <c r="H34" s="32"/>
+      <c r="F34" s="31"/>
+      <c r="G34" s="31"/>
+      <c r="H34" s="31"/>
       <c r="I34" s="24"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="21"/>
       <c r="B35" s="22"/>
-      <c r="D35" s="33"/>
+      <c r="D35" s="32"/>
       <c r="E35" s="23"/>
-      <c r="F35" s="32"/>
-      <c r="G35" s="32"/>
-      <c r="H35" s="32"/>
+      <c r="F35" s="31"/>
+      <c r="G35" s="31"/>
+      <c r="H35" s="31"/>
       <c r="I35" s="24"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="21"/>
       <c r="B36" s="22"/>
-      <c r="D36" s="33"/>
+      <c r="D36" s="32"/>
       <c r="E36" s="23"/>
-      <c r="F36" s="32"/>
-      <c r="G36" s="32"/>
-      <c r="H36" s="32"/>
+      <c r="F36" s="31"/>
+      <c r="G36" s="31"/>
+      <c r="H36" s="31"/>
       <c r="I36" s="24"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="21"/>
       <c r="B37" s="22"/>
-      <c r="D37" s="33"/>
+      <c r="D37" s="32"/>
       <c r="E37" s="23"/>
-      <c r="F37" s="32"/>
-      <c r="G37" s="32"/>
-      <c r="H37" s="32"/>
+      <c r="F37" s="31"/>
+      <c r="G37" s="31"/>
+      <c r="H37" s="31"/>
       <c r="I37" s="24"/>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finished event table notes
</commit_message>
<xml_diff>
--- a/Event Table/EventTable.xlsx
+++ b/Event Table/EventTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nagoya\Documents\Uni\Semester 2\SAM 2021\modellingAssignment1\Event Table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9F45F7B-1818-43D6-8AF1-F7F56D6ADF1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12719ED5-A181-49CD-A3F8-D5969FED00E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{32C6574B-FC3F-4F92-B702-88451B0D3896}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="32220" windowHeight="19635" xr2:uid="{32C6574B-FC3F-4F92-B702-88451B0D3896}"/>
   </bookViews>
   <sheets>
     <sheet name="eventTable" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="150">
   <si>
     <t>Event Name</t>
   </si>
@@ -480,6 +480,24 @@
   </si>
   <si>
     <t>Confirm bank has received funds, store value in the system</t>
+  </si>
+  <si>
+    <t>Used for withholding security deposits in the event that a customer returns a pack in a damaged or incomplete state</t>
+  </si>
+  <si>
+    <t>Catches the possibility of a declined payment</t>
+  </si>
+  <si>
+    <t>Charges the customer when they have requested to hire an equipment pack</t>
+  </si>
+  <si>
+    <t>This event is for specifically marking that a pack has been collected by a customer after they have paid their hire fee and deposit</t>
+  </si>
+  <si>
+    <t>Clearly marks the pack as being returned to a storage location</t>
+  </si>
+  <si>
+    <t>This event enables the bank to send relevant transaction information to the ATO (see Rich Picture)</t>
   </si>
 </sst>
 </file>
@@ -1090,7 +1108,7 @@
   <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1334,7 +1352,9 @@
       <c r="H8" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="I8" s="35"/>
+      <c r="I8" s="28" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="9" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="36" t="s">
@@ -1361,7 +1381,9 @@
       <c r="H9" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="I9" s="35"/>
+      <c r="I9" s="28" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="36" t="s">
@@ -1388,7 +1410,9 @@
       <c r="H10" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="I10" s="35"/>
+      <c r="I10" s="35" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="11" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="36" t="s">
@@ -1415,7 +1439,9 @@
       <c r="H11" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="I11" s="35"/>
+      <c r="I11" s="28" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="36" t="s">
@@ -1442,7 +1468,9 @@
       <c r="H12" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="I12" s="35"/>
+      <c r="I12" s="35" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="13" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="36" t="s">
@@ -1469,7 +1497,9 @@
       <c r="H13" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="I13" s="35"/>
+      <c r="I13" s="28" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="14" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="36" t="s">
@@ -1496,7 +1526,9 @@
       <c r="H14" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="I14" s="35"/>
+      <c r="I14" s="35" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="15" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="36" t="s">
@@ -1523,7 +1555,9 @@
       <c r="H15" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="I15" s="35"/>
+      <c r="I15" s="28" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="16" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="36" t="s">
@@ -1550,7 +1584,9 @@
       <c r="H16" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="I16" s="35"/>
+      <c r="I16" s="35" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="17" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="36" t="s">
@@ -1577,7 +1613,9 @@
       <c r="H17" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="I17" s="35"/>
+      <c r="I17" s="35" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="18" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="36" t="s">
@@ -1604,7 +1642,9 @@
       <c r="H18" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="I18" s="35"/>
+      <c r="I18" s="28" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="19" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="36" t="s">
@@ -1631,7 +1671,9 @@
       <c r="H19" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="I19" s="35"/>
+      <c r="I19" s="28" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="20" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="36" t="s">
@@ -1658,7 +1700,9 @@
       <c r="H20" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="I20" s="35"/>
+      <c r="I20" s="28" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="21" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="36" t="s">
@@ -1685,7 +1729,9 @@
       <c r="H21" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="I21" s="35"/>
+      <c r="I21" s="28" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="22" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="36" t="s">
@@ -1712,7 +1758,9 @@
       <c r="H22" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="I22" s="35"/>
+      <c r="I22" s="35" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="21"/>

</xml_diff>

<commit_message>
did a lot of work and fixed a lot of formatting
</commit_message>
<xml_diff>
--- a/Event Table/EventTable.xlsx
+++ b/Event Table/EventTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nagoya\Documents\Uni\Semester 2\SAM 2021\modellingAssignment1\Event Table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12719ED5-A181-49CD-A3F8-D5969FED00E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{699E87CC-F8AA-4CDB-BFA2-028B024FBDEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="32220" windowHeight="19635" xr2:uid="{32C6574B-FC3F-4F92-B702-88451B0D3896}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21000" xr2:uid="{32C6574B-FC3F-4F92-B702-88451B0D3896}"/>
   </bookViews>
   <sheets>
     <sheet name="eventTable" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="159">
   <si>
     <t>Event Name</t>
   </si>
@@ -498,6 +498,36 @@
   </si>
   <si>
     <t>This event enables the bank to send relevant transaction information to the ATO (see Rich Picture)</t>
+  </si>
+  <si>
+    <t>Combine Incomplete Packs</t>
+  </si>
+  <si>
+    <t>Generate Pack Condition Report</t>
+  </si>
+  <si>
+    <t>One or more of the same pack type is incomplete and can be combined to make one complete and undamaged pack</t>
+  </si>
+  <si>
+    <t>1. Two Equipment Packs are combined if they both share the parameter "Incomplete/Damaged"
+2. One Equipment Pack of the same kind is created and has the parameter "Complete/Undamaged"
+3. The other "Incomplete/Damaged" Equipment Pack is deleted from the system</t>
+  </si>
+  <si>
+    <t>Merge Equipment Packs</t>
+  </si>
+  <si>
+    <t>Storage Location</t>
+  </si>
+  <si>
+    <t>The day is a Friday</t>
+  </si>
+  <si>
+    <t>1. Aggregate all most recent equipment state data
+2. Generate and display a report</t>
+  </si>
+  <si>
+    <t>Report is generated and displayed to Management and Customer Interactions</t>
   </si>
 </sst>
 </file>
@@ -1105,10 +1135,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{691D4392-63F1-4651-BDBD-40240F036054}">
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1619,10 +1649,10 @@
     </row>
     <row r="18" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="B18" s="25" t="s">
-        <v>9</v>
+        <v>150</v>
+      </c>
+      <c r="B18" s="26" t="s">
+        <v>15</v>
       </c>
       <c r="C18" s="28" t="s">
         <v>10</v>
@@ -1630,17 +1660,17 @@
       <c r="D18" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="E18" s="40" t="s">
-        <v>93</v>
+      <c r="E18" s="35" t="s">
+        <v>152</v>
       </c>
       <c r="F18" s="35" t="s">
-        <v>132</v>
+        <v>153</v>
       </c>
       <c r="G18" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="H18" s="28" t="s">
-        <v>10</v>
+        <v>154</v>
+      </c>
+      <c r="H18" s="34" t="s">
+        <v>155</v>
       </c>
       <c r="I18" s="28" t="s">
         <v>10</v>
@@ -1648,7 +1678,7 @@
     </row>
     <row r="19" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="36" t="s">
-        <v>78</v>
+        <v>151</v>
       </c>
       <c r="B19" s="25" t="s">
         <v>9</v>
@@ -1659,23 +1689,23 @@
       <c r="D19" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="40" t="s">
-        <v>99</v>
+      <c r="E19" s="35" t="s">
+        <v>156</v>
       </c>
       <c r="F19" s="35" t="s">
-        <v>133</v>
+        <v>157</v>
       </c>
       <c r="G19" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="H19" s="28" t="s">
-        <v>10</v>
+        <v>158</v>
+      </c>
+      <c r="H19" s="34" t="s">
+        <v>142</v>
       </c>
       <c r="I19" s="28" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="36" t="s">
         <v>78</v>
       </c>
@@ -1689,10 +1719,10 @@
         <v>10</v>
       </c>
       <c r="E20" s="40" t="s">
-        <v>125</v>
+        <v>93</v>
       </c>
       <c r="F20" s="35" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G20" s="28" t="s">
         <v>10</v>
@@ -1706,7 +1736,7 @@
     </row>
     <row r="21" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="36" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B21" s="25" t="s">
         <v>9</v>
@@ -1718,76 +1748,113 @@
         <v>10</v>
       </c>
       <c r="E21" s="40" t="s">
+        <v>99</v>
+      </c>
+      <c r="F21" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="G21" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="H21" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="I21" s="28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="B22" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="F22" s="35" t="s">
+        <v>134</v>
+      </c>
+      <c r="G22" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="I22" s="28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="40" t="s">
         <v>100</v>
       </c>
-      <c r="F21" s="35" t="s">
+      <c r="F23" s="35" t="s">
         <v>135</v>
       </c>
-      <c r="G21" s="40" t="s">
+      <c r="G23" s="40" t="s">
         <v>140</v>
       </c>
-      <c r="H21" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="I21" s="28" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="36" t="s">
+      <c r="H23" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="I23" s="28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="B22" s="26" t="s">
+      <c r="B24" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="E22" s="35" t="s">
+      <c r="C24" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="F22" s="35" t="s">
+      <c r="F24" s="35" t="s">
         <v>126</v>
       </c>
-      <c r="G22" s="40" t="s">
+      <c r="G24" s="40" t="s">
         <v>141</v>
       </c>
-      <c r="H22" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="I22" s="35" t="s">
+      <c r="H24" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="I24" s="35" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="21"/>
-      <c r="B23" s="22"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="31"/>
-      <c r="G23" s="31"/>
-      <c r="H23" s="31"/>
-      <c r="I23" s="24"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="21"/>
-      <c r="B24" s="22"/>
-      <c r="C24" s="23"/>
-      <c r="D24" s="32"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="31"/>
-      <c r="I24" s="24"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="21"/>
       <c r="B25" s="22"/>
-      <c r="D25" s="32"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
       <c r="E25" s="23"/>
       <c r="F25" s="31"/>
       <c r="G25" s="31"/>
@@ -1795,51 +1862,52 @@
       <c r="I25" s="24"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="37"/>
-      <c r="B26" s="32"/>
-      <c r="C26" s="38"/>
-      <c r="D26" s="38"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="39"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="39"/>
-      <c r="I26" s="39"/>
+      <c r="A26" s="21"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="31"/>
+      <c r="I26" s="24"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="37"/>
-      <c r="B27" s="32"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="39"/>
-      <c r="G27" s="39"/>
-      <c r="H27" s="39"/>
-      <c r="I27" s="39"/>
+      <c r="A27" s="21"/>
+      <c r="B27" s="22"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="24"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="21"/>
-      <c r="B28" s="22"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="31"/>
-      <c r="I28" s="24"/>
+      <c r="A28" s="37"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="39"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="39"/>
+      <c r="I28" s="39"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="21"/>
-      <c r="B29" s="22"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="24"/>
+      <c r="A29" s="37"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="21"/>
       <c r="B30" s="22"/>
-      <c r="D30" s="32"/>
+      <c r="D30" s="23"/>
       <c r="E30" s="23"/>
       <c r="F30" s="31"/>
       <c r="G30" s="31"/>
@@ -1859,7 +1927,7 @@
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="21"/>
       <c r="B32" s="22"/>
-      <c r="D32" s="23"/>
+      <c r="D32" s="32"/>
       <c r="E32" s="23"/>
       <c r="F32" s="31"/>
       <c r="G32" s="31"/>
@@ -1869,7 +1937,7 @@
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="21"/>
       <c r="B33" s="22"/>
-      <c r="D33" s="32"/>
+      <c r="D33" s="23"/>
       <c r="E33" s="23"/>
       <c r="F33" s="31"/>
       <c r="G33" s="31"/>
@@ -1879,7 +1947,7 @@
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="21"/>
       <c r="B34" s="22"/>
-      <c r="D34" s="32"/>
+      <c r="D34" s="23"/>
       <c r="E34" s="23"/>
       <c r="F34" s="31"/>
       <c r="G34" s="31"/>
@@ -1916,8 +1984,28 @@
       <c r="H37" s="31"/>
       <c r="I37" s="24"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="21"/>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="21"/>
+      <c r="B38" s="22"/>
+      <c r="D38" s="32"/>
+      <c r="E38" s="23"/>
+      <c r="F38" s="31"/>
+      <c r="G38" s="31"/>
+      <c r="H38" s="31"/>
+      <c r="I38" s="24"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="21"/>
+      <c r="B39" s="22"/>
+      <c r="D39" s="32"/>
+      <c r="E39" s="23"/>
+      <c r="F39" s="31"/>
+      <c r="G39" s="31"/>
+      <c r="H39" s="31"/>
+      <c r="I39" s="24"/>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>